<commit_message>
Update 2025 budget with actual spending data from Open Collective
Analyzed 348 transactions from opencollective.com/policyengine:
- 181 expense transactions in 2025
- YTD spending (Jan-Oct): $470,611
- Annualized projection: $564,734

Expense breakdown based on actual spending:
- Fellowships & Internships: $103,904 (18.4%)
- PolicyEngine UK Operations: $100,965 (17.9%)
- Contractor Services: $94,170 (16.7%)
- Cloud Infrastructure: $68,868 (12.2%)
- Website Development: $36,000 (6.4%)
- Travel & Conferences: $28,751 (5.1%)
- Payroll: $22,021 (3.9%)
- Other categories: <3% each

Note: OC shows $1.1M estimated annual budget, but actual spending
projects to ~$565k. Budget reflects actual spending patterns from
real transaction data.

Data: policyengine-transactions.csv (348 transactions)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/financials/PolicyEngine_Current_Year_Budget_2025.xlsx
+++ b/financials/PolicyEngine_Current_Year_Budget_2025.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FY2026 Budget" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2025 Budget" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="$#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,6 +41,9 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <i val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -69,7 +72,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -78,6 +81,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -443,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,9 +458,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,247 +473,296 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Current Year Budget: Calendar Year 2025 (Estimated Annual)</t>
+          <t>Calendar Year 2025 Budget (Actual Spending Through October)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Data source: opencollective.com/policyengine</t>
+          <t>Data source: opencollective.com/policyengine (348 transactions analyzed)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>Estimated Annual Budget</t>
+          <t>Year-to-Date Actuals (Jan-Oct 2025)</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>1100315</v>
+        <v>470611</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Annualized Projection (12 months)</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>564734</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
-        <is>
-          <t>REVENUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Foundation Grants</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>900000</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Major foundation support</t>
-        </is>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Current Balance (Oct 2025)</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>545558</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Individual Contributions</t>
-        </is>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>50000</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Open Collective donors</t>
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>EXPENSE BREAKDOWN (Annualized)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Institutional Partnerships</t>
+          <t>Fellowships &amp; Internships</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>100000</v>
+        <v>103904</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Research collaborations</t>
+          <t>18.4%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Other Income</t>
+          <t>PolicyEngine UK Operations</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>50315</v>
+        <v>100965</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Miscellaneous revenue</t>
+          <t>17.9%</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>TOTAL REVENUE</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="n">
-        <v>1100315</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Contractor Services</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>94170</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>16.7%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Cloud Infrastructure</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>68868</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12.2%</t>
+        </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
-        <is>
-          <t>EXPENSES</t>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Website Development</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>36000</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>6.4%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Salaries &amp; Benefits</t>
+          <t>Travel &amp; Conferences</t>
         </is>
       </c>
       <c r="B15" s="5" t="n">
-        <v>650000</v>
+        <v>28751</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Core technical and policy staff</t>
+          <t>5.1%</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Contractor Payments</t>
+          <t>Payroll Expenses</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>250000</v>
+        <v>22021</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Specialized expertise and development</t>
+          <t>3.9%</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Software &amp; Infrastructure</t>
+          <t>Legal Services</t>
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>80000</v>
+        <v>13878</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cloud hosting, tools, licenses</t>
+          <t>2.5%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Professional Services</t>
+          <t>AI/Software Subscriptions</t>
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>40000</v>
+        <v>10145</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Legal, accounting, consulting</t>
+          <t>1.8%</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Travel &amp; Events</t>
+          <t>Equipment &amp; Materials</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>20000</v>
+        <v>7994</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Conferences, meetings, training</t>
+          <t>1.4%</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Marketing &amp; Communications</t>
+          <t>Office Space</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>15000</v>
+        <v>6672</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Outreach and user acquisition</t>
+          <t>1.2%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Other Operating Expenses</t>
+          <t>Events &amp; Supplies</t>
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>45315</v>
+        <v>1683</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Office supplies, insurance, miscellaneous</t>
+          <t>0.3%</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>TOTAL EXPENSES</t>
-        </is>
-      </c>
-      <c r="B22" s="7" t="n">
-        <v>1100315</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="inlineStr">
-        <is>
-          <t>PROJECTED NET INCOME</t>
-        </is>
-      </c>
-      <c r="B24" s="7" t="n">
-        <v>0</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Other Operating</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>69683</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>12.3%</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>TOTAL EXPENSES (Annualized)</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="n">
+        <v>564734</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>REVENUE (YTD Jan-Oct 2025)</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Current Balance (as of October 2025)</t>
+          <t>Foundation Grants &amp; Contributions</t>
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>545558</v>
-      </c>
-    </row>
+        <v>643910</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>Note:</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9" t="inlineStr">
+        <is>
+          <t>Open Collective shows estimated annual budget of $1,100,315, but actual spending through October 2025 totals $470,611 (10 months), projecting to ~$565,000 annualized. This budget reflects actual spending patterns. The difference may reflect planned but not yet executed activities or conservative budgeting.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30"/>
+    <row r="31"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A29:C31"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>